<commit_message>
Updated with scatter chart.
--HG--
branch : feature/Pie_Chart
</commit_message>
<xml_diff>
--- a/openpyxl/sample/files/charts_gen.xlsx
+++ b/openpyxl/sample/files/charts_gen.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Dates" r:id="rId4" sheetId="4"/>
     <sheet name="Pie" r:id="rId5" sheetId="5"/>
     <sheet name="Line" r:id="rId6" sheetId="6"/>
+    <sheet name="Scatter" r:id="rId7" sheetId="7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -905,6 +906,157 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.03375"/>
+          <c:y val="0.31"/>
+          <c:w val="0.6"/>
+          <c:h val="0.6"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Scatter'!$B$1:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Scatter'!$A$1:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="60871424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="90.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60873344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10.0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="60873344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60871424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2.0"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.75"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
@@ -1031,6 +1183,31 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="95250" y="3810000"/>
+    <xdr:ext cx="7620000" cy="3810000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
@@ -1787,4 +1964,106 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col max="1" collapsed="0" width="9.10" min="1"/>
+    <col max="2" collapsed="0" width="9.10" min="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>